<commit_message>
Author:Akash Description:modified xls Sheet file:Akash.xlsx
</commit_message>
<xml_diff>
--- a/TeamDetails/TasksBreakDown/Akash.xlsx
+++ b/TeamDetails/TasksBreakDown/Akash.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Internship_2017\trunk\TeamDetails\TasksBreakDown\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Akash Sharma\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="32">
   <si>
     <t>Story ID</t>
   </si>
@@ -122,6 +122,9 @@
   <si>
     <t>SSDMS-13(submit button)</t>
   </si>
+  <si>
+    <t>HOUR NEEDED</t>
+  </si>
 </sst>
 </file>
 
@@ -144,7 +147,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +181,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -246,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -282,6 +297,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2885,8 +2902,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2934,8 +2951,8 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="9"/>
-      <c r="B3" s="18">
-        <v>30</v>
+      <c r="B3" s="20">
+        <v>24</v>
       </c>
       <c r="C3" s="10" t="s">
         <v>11</v>
@@ -2955,10 +2972,10 @@
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="19"/>
+      <c r="B4" s="21"/>
       <c r="C4" s="10" t="s">
         <v>13</v>
       </c>
@@ -2977,8 +2994,8 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="19"/>
+      <c r="A5" s="21"/>
+      <c r="B5" s="21"/>
       <c r="C5" s="10" t="s">
         <v>15</v>
       </c>
@@ -2997,8 +3014,8 @@
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="19"/>
+      <c r="A6" s="21"/>
+      <c r="B6" s="21"/>
       <c r="C6" s="10" t="s">
         <v>16</v>
       </c>
@@ -3009,16 +3026,16 @@
         <v>7</v>
       </c>
       <c r="F6" s="10">
+        <v>4</v>
+      </c>
+      <c r="G6" s="10">
         <v>3</v>
       </c>
-      <c r="G6" s="10">
-        <v>4</v>
-      </c>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="19"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="10" t="s">
         <v>18</v>
       </c>
@@ -3029,16 +3046,16 @@
         <v>7</v>
       </c>
       <c r="F7" s="10">
+        <v>4</v>
+      </c>
+      <c r="G7" s="10">
         <v>3</v>
       </c>
-      <c r="G7" s="10">
-        <v>4</v>
-      </c>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="19"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="10" t="s">
         <v>20</v>
       </c>
@@ -3046,17 +3063,19 @@
         <v>21</v>
       </c>
       <c r="E8" s="10">
-        <v>2</v>
-      </c>
-      <c r="F8" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
       <c r="G8" s="10">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="19"/>
+      <c r="A9" s="21"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="10" t="s">
         <v>22</v>
       </c>
@@ -3064,17 +3083,17 @@
         <v>23</v>
       </c>
       <c r="E9" s="10">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F9" s="10"/>
       <c r="G9" s="10">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="19"/>
+      <c r="A10" s="21"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="10" t="s">
         <v>24</v>
       </c>
@@ -3091,8 +3110,8 @@
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="19"/>
+      <c r="A11" s="21"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="10" t="s">
         <v>25</v>
       </c>
@@ -3109,8 +3128,8 @@
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
+      <c r="A12" s="21"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="10" t="s">
         <v>26</v>
       </c>
@@ -3127,23 +3146,25 @@
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20"/>
+      <c r="A13" s="21"/>
+      <c r="B13" s="22"/>
       <c r="C13" s="10"/>
       <c r="D13" s="11"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="10">
-        <v>1</v>
-      </c>
+      <c r="E13" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F13" s="18">
+        <v>13</v>
+      </c>
+      <c r="G13" s="10"/>
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
+      <c r="A14" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="21">
-        <v>30</v>
+      <c r="B14" s="23">
+        <v>18</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>11</v>
@@ -3152,17 +3173,17 @@
         <v>12</v>
       </c>
       <c r="E14" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F14" s="12"/>
       <c r="G14" s="12">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="22"/>
-      <c r="B15" s="22"/>
+      <c r="A15" s="24"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="12" t="s">
         <v>13</v>
       </c>
@@ -3170,17 +3191,17 @@
         <v>14</v>
       </c>
       <c r="E15" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="22"/>
-      <c r="B16" s="22"/>
+      <c r="A16" s="24"/>
+      <c r="B16" s="24"/>
       <c r="C16" s="12" t="s">
         <v>15</v>
       </c>
@@ -3188,17 +3209,17 @@
         <v>10</v>
       </c>
       <c r="E16" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="22"/>
-      <c r="B17" s="22"/>
+      <c r="A17" s="24"/>
+      <c r="B17" s="24"/>
       <c r="C17" s="12" t="s">
         <v>16</v>
       </c>
@@ -3206,17 +3227,17 @@
         <v>17</v>
       </c>
       <c r="E17" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F17" s="12"/>
       <c r="G17" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="22"/>
-      <c r="B18" s="22"/>
+      <c r="A18" s="24"/>
+      <c r="B18" s="24"/>
       <c r="C18" s="12" t="s">
         <v>18</v>
       </c>
@@ -3224,17 +3245,17 @@
         <v>19</v>
       </c>
       <c r="E18" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F18" s="12"/>
       <c r="G18" s="12">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="22"/>
-      <c r="B19" s="22"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="24"/>
       <c r="C19" s="12" t="s">
         <v>20</v>
       </c>
@@ -3242,17 +3263,17 @@
         <v>27</v>
       </c>
       <c r="E19" s="12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F19" s="12"/>
       <c r="G19" s="12">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="22"/>
-      <c r="B20" s="22"/>
+      <c r="A20" s="24"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="12" t="s">
         <v>22</v>
       </c>
@@ -3269,8 +3290,8 @@
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="22"/>
-      <c r="B21" s="22"/>
+      <c r="A21" s="24"/>
+      <c r="B21" s="24"/>
       <c r="C21" s="12" t="s">
         <v>24</v>
       </c>
@@ -3287,8 +3308,8 @@
       <c r="H21" s="8"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="22"/>
-      <c r="B22" s="22"/>
+      <c r="A22" s="24"/>
+      <c r="B22" s="24"/>
       <c r="C22" s="12" t="s">
         <v>25</v>
       </c>
@@ -3305,8 +3326,8 @@
       <c r="H22" s="8"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="22"/>
-      <c r="B23" s="22"/>
+      <c r="A23" s="24"/>
+      <c r="B23" s="24"/>
       <c r="C23" s="12" t="s">
         <v>26</v>
       </c>
@@ -3323,25 +3344,27 @@
       <c r="H23" s="8"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
+      <c r="A24" s="25"/>
+      <c r="B24" s="25"/>
       <c r="C24" s="12"/>
       <c r="D24" s="13"/>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
-      <c r="G24" s="12">
-        <v>1</v>
-      </c>
+      <c r="G24" s="12"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
-      <c r="G25" s="2">
-        <f t="shared" ref="G25:G26" si="0">E25-F25</f>
-        <v>0</v>
+      <c r="E25" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="18">
+        <v>16</v>
+      </c>
+      <c r="G25" s="2" t="e">
+        <f>E25-F25</f>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3351,7 +3374,7 @@
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
       <c r="G26" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="G26" si="0">E26-F26</f>
         <v>0</v>
       </c>
     </row>
@@ -3378,7 +3401,7 @@
       <c r="I28" s="15"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="17"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="15"/>
       <c r="C29" s="15"/>
       <c r="D29" s="16"/>
@@ -3389,7 +3412,7 @@
       <c r="I29" s="15"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A30" s="17"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="15"/>
       <c r="C30" s="15"/>
       <c r="D30" s="16"/>
@@ -3400,7 +3423,7 @@
       <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="17"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="15"/>
       <c r="C31" s="15"/>
       <c r="D31" s="16"/>
@@ -3411,7 +3434,7 @@
       <c r="I31" s="15"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="17"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="15"/>
       <c r="C32" s="15"/>
       <c r="D32" s="16"/>
@@ -3422,7 +3445,7 @@
       <c r="I32" s="15"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="17"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="15"/>
       <c r="C33" s="15"/>
       <c r="D33" s="16"/>
@@ -3433,7 +3456,7 @@
       <c r="I33" s="15"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="17"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="15"/>
       <c r="C34" s="15"/>
       <c r="D34" s="16"/>
@@ -3444,7 +3467,7 @@
       <c r="I34" s="15"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="17"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="16"/>
@@ -3455,7 +3478,7 @@
       <c r="I35" s="15"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A36" s="17"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="16"/>
@@ -3466,7 +3489,7 @@
       <c r="I36" s="15"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="17"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="15"/>
       <c r="C37" s="15"/>
       <c r="D37" s="16"/>
@@ -3477,7 +3500,7 @@
       <c r="I37" s="15"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="15"/>
       <c r="C38" s="15"/>
       <c r="D38" s="16"/>
@@ -3488,7 +3511,7 @@
       <c r="I38" s="15"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A39" s="17"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="16"/>
@@ -3499,7 +3522,7 @@
       <c r="I39" s="15"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A40" s="17"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="16"/>
@@ -3510,7 +3533,7 @@
       <c r="I40" s="15"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A41" s="17"/>
+      <c r="A41" s="19"/>
       <c r="B41" s="15"/>
       <c r="C41" s="15"/>
       <c r="D41" s="16"/>
@@ -3521,7 +3544,7 @@
       <c r="I41" s="15"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A42" s="17"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="15"/>
       <c r="C42" s="15"/>
       <c r="D42" s="16"/>
@@ -3532,7 +3555,7 @@
       <c r="I42" s="15"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A43" s="17"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="15"/>
       <c r="C43" s="15"/>
       <c r="D43" s="16"/>
@@ -3543,7 +3566,7 @@
       <c r="I43" s="15"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A44" s="17"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="15"/>
       <c r="C44" s="15"/>
       <c r="D44" s="16"/>
@@ -3554,7 +3577,7 @@
       <c r="I44" s="15"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A45" s="17"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="15"/>
       <c r="C45" s="15"/>
       <c r="D45" s="16"/>

</xml_diff>